<commit_message>
fixed display operation with USB disconnected
When USB disconnected on an Arduino Nano Every, the nexInit() doesn't complete properly. After every command the recRecCommandFinished() driver function waits for a display response until the 100ms timeout is reached.

Resend     sendCommand("bkcmd=1"); when exiting the splash page to fix.
</commit_message>
<xml_diff>
--- a/documentation/sensor calibration and lookup table.xlsx
+++ b/documentation/sensor calibration and lookup table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d529807eb1393ed/documents/amateur radio/projects/kjell VSWR/github/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d529807eb1393ed/documents/amateur radio/projects/Log-VSWR-Bridge/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{F44F183F-E7B5-45D9-8CF5-4FBDF6E67F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{193E94D9-4BC0-4E49-9965-344C5529F4D3}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{F44F183F-E7B5-45D9-8CF5-4FBDF6E67F76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E536E566-4726-413D-B205-71D5D053F732}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E06A0820-D64A-4C60-B12F-38E92E047173}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:P1032"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4327,7 +4327,7 @@
         <v>2.2446053936589276</v>
       </c>
       <c r="P74" t="str">
-        <f t="shared" ref="P74:P136" si="9">_xlfn.CONCAT(ROUND(G74,5),",",ROUND(H74,5),",",ROUND(I74,5),",",ROUND(J74,5),",",ROUND(K74,5),",",ROUND(L74,5),",",ROUND(M74,5),",",ROUND(N74,5),",")</f>
+        <f t="shared" ref="P74:P135" si="9">_xlfn.CONCAT(ROUND(G74,5),",",ROUND(H74,5),",",ROUND(I74,5),",",ROUND(J74,5),",",ROUND(K74,5),",",ROUND(L74,5),",",ROUND(M74,5),",",ROUND(N74,5),",")</f>
         <v>2.02901,2.0585,2.08841,2.11875,2.14954,2.18077,2.21246,2.24461,</v>
       </c>
     </row>

</xml_diff>